<commit_message>
Added check_delta to the simple example
</commit_message>
<xml_diff>
--- a/examples/simple/simple.xlsx
+++ b/examples/simple/simple.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kaklise\src\pecos\examples\simple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kaklise\src\Pecos\pecos\examples\simple\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2DC5FD-C5A2-4855-A794-83D0EB993A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -579,7 +580,7 @@
                   <c:v>0.47916666655510198</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.48958333321934333</c:v>
+                  <c:v>0.488583333219343</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0.50004318117923363</c:v>
@@ -2988,7 +2989,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3328,11 +3335,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49:H60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4143,7 +4150,7 @@
         <v>42005.489583333219</v>
       </c>
       <c r="B48" s="5">
-        <v>0.48958333321934333</v>
+        <v>0.488583333219343</v>
       </c>
       <c r="C48">
         <v>0.86213256517154802</v>
@@ -4989,7 +4996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5001,7 +5008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>